<commit_message>
cambios en generacion de archivos
</commit_message>
<xml_diff>
--- a/VTT Tool/VTT DATA.xlsx
+++ b/VTT Tool/VTT DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OLMEDOJorge\Documents\Python projects\Horse Luis\VTT Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D410B4-BC15-4846-B24E-D8ACB2AECE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF889D0A-9303-4D6F-A97C-99D06B01A63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F9BAF1D-C4F9-4C63-99BA-ADCB8DC6383A}"/>
   </bookViews>
@@ -2556,10 +2556,10 @@
   <dimension ref="A1:BD51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="AR2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="L5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BA1" sqref="BA1"/>
+      <selection pane="bottomRight" activeCell="A51" sqref="A51:XFD51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12257,7 +12257,7 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
   <autoFilter ref="A1:BD51" xr:uid="{869D9611-F0E3-4A7A-9239-9C1FA0F0C8DA}"/>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="A51 A2:BC2 C51:AZ51 A3:AZ50 BA3:BC51">
+  <conditionalFormatting sqref="A2:BC2 A3:AZ50 BA3:BC51 A51 C51:AZ51">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$BD2&lt;=TODAY()</formula>
     </cfRule>

</xml_diff>

<commit_message>
se agrego camiones nuevamente
</commit_message>
<xml_diff>
--- a/VTT Tool/VTT DATA.xlsx
+++ b/VTT Tool/VTT DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OLMEDOJorge\Documents\Python projects\Horse Luis\VTT Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C041BB-17AA-4EF6-B742-8BA82977C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CE09E7-E082-4862-B417-FA2F899F1F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F9BAF1D-C4F9-4C63-99BA-ADCB8DC6383A}"/>
   </bookViews>
@@ -2556,10 +2556,10 @@
   <dimension ref="A1:BD51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AC8" sqref="AC8"/>
+      <selection pane="bottomRight" activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
dias abreviados y quite 16 manufacturing
</commit_message>
<xml_diff>
--- a/VTT Tool/VTT DATA.xlsx
+++ b/VTT Tool/VTT DATA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OLMEDOJorge\Documents\Python projects\Horse Luis\VTT Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E9F99A-D912-419B-A4F2-1EED93DA787D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B625301-F6F2-4413-8C13-0B4C7EBA3F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F9BAF1D-C4F9-4C63-99BA-ADCB8DC6383A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="VTT actif" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VTT actif'!$A$1:$BD$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'VTT actif'!$A$1:$BD$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1123,14 +1123,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{432BBFD9-EC83-40A5-8B27-79052821547A}"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1460,16 +1453,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{869D9611-F0E3-4A7A-9239-9C1FA0F0C8DA}">
-  <sheetPr codeName="Feuil4">
+  <sheetPr codeName="Feuil4" filterMode="1">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:BD51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="11" ySplit="1" topLeftCell="AP20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="1" topLeftCell="AN48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AY52" sqref="AY52"/>
+      <selection pane="bottomRight" activeCell="AP48" sqref="AP48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,7 +1658,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>416</v>
       </c>
@@ -1855,7 +1848,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>901</v>
       </c>
@@ -1941,7 +1934,7 @@
         <v>26</v>
       </c>
       <c r="Z3" s="7">
-        <f t="shared" ref="Z3:Z51" si="19">+Y3+X3-1</f>
+        <f t="shared" ref="Z3:Z50" si="19">+Y3+X3-1</f>
         <v>30</v>
       </c>
       <c r="AA3" s="7">
@@ -2045,7 +2038,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>916</v>
       </c>
@@ -2235,7 +2228,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>752</v>
       </c>
@@ -2425,7 +2418,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>761</v>
       </c>
@@ -2615,7 +2608,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>927</v>
       </c>
@@ -2805,7 +2798,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>930</v>
       </c>
@@ -2995,7 +2988,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>931</v>
       </c>
@@ -3185,7 +3178,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>932</v>
       </c>
@@ -3375,7 +3368,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <v>1027</v>
       </c>
@@ -3565,7 +3558,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>1045</v>
       </c>
@@ -3755,7 +3748,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>1060</v>
       </c>
@@ -3945,7 +3938,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>233</v>
       </c>
@@ -4136,7 +4129,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>928</v>
       </c>
@@ -4326,7 +4319,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>926</v>
       </c>
@@ -4516,7 +4509,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>981</v>
       </c>
@@ -4706,7 +4699,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>120</v>
       </c>
@@ -4896,7 +4889,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>915</v>
       </c>
@@ -5086,7 +5079,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>917</v>
       </c>
@@ -5276,7 +5269,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>918</v>
       </c>
@@ -5466,7 +5459,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>925</v>
       </c>
@@ -5656,7 +5649,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>121</v>
       </c>
@@ -5846,7 +5839,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>912</v>
       </c>
@@ -6036,7 +6029,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>920</v>
       </c>
@@ -6226,7 +6219,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>921</v>
       </c>
@@ -6416,7 +6409,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>1001</v>
       </c>
@@ -6606,7 +6599,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>1063</v>
       </c>
@@ -6796,7 +6789,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>1005</v>
       </c>
@@ -6986,7 +6979,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>1006</v>
       </c>
@@ -7176,7 +7169,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>1007</v>
       </c>
@@ -7366,7 +7359,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>1008</v>
       </c>
@@ -7556,7 +7549,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="33" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>1009</v>
       </c>
@@ -7746,7 +7739,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="34" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>1010</v>
       </c>
@@ -7936,7 +7929,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="35" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>1012</v>
       </c>
@@ -8126,7 +8119,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="36" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>1034</v>
       </c>
@@ -8316,7 +8309,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="37" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>1037</v>
       </c>
@@ -8506,7 +8499,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="38" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>1040</v>
       </c>
@@ -8696,7 +8689,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="39" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>1029</v>
       </c>
@@ -8886,7 +8879,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="40" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>1032</v>
       </c>
@@ -9076,7 +9069,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="41" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>1033</v>
       </c>
@@ -9266,7 +9259,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="42" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>904</v>
       </c>
@@ -9456,7 +9449,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="43" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>906</v>
       </c>
@@ -9646,7 +9639,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="44" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>924</v>
       </c>
@@ -9836,7 +9829,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="45" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>1014</v>
       </c>
@@ -10026,7 +10019,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="46" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>1015</v>
       </c>
@@ -10216,7 +10209,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="47" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>1036</v>
       </c>
@@ -10485,19 +10478,19 @@
         <v>31</v>
       </c>
       <c r="X48" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Y48" s="4">
         <f t="shared" si="28"/>
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Z48" s="7">
-        <f t="shared" si="19"/>
-        <v>29</v>
+        <f>+Y48+X48-6</f>
+        <v>38</v>
       </c>
       <c r="AA48" s="7">
         <f t="shared" si="29"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="AB48" s="4">
         <v>3</v>
@@ -10513,21 +10506,21 @@
       </c>
       <c r="AF48" s="4">
         <f t="shared" si="30"/>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="AG48" s="7">
         <v>3</v>
       </c>
       <c r="AH48" s="7">
         <f t="shared" si="31"/>
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AI48" s="4">
         <v>0</v>
       </c>
       <c r="AJ48" s="4">
         <f t="shared" si="32"/>
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="AK48" s="4" t="s">
         <v>81</v>
@@ -10537,36 +10530,36 @@
       </c>
       <c r="AM48" s="4">
         <f t="shared" si="33"/>
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="AN48" s="4">
         <v>2</v>
       </c>
       <c r="AO48" s="4">
         <f t="shared" si="34"/>
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="AP48" s="4">
         <v>3</v>
       </c>
       <c r="AQ48" s="4">
         <f t="shared" si="35"/>
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="AR48" s="4">
         <f t="shared" si="36"/>
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="AS48" s="4">
         <f t="shared" si="37"/>
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="AT48" s="4">
         <v>0</v>
       </c>
       <c r="AU48" s="4">
         <f t="shared" si="38"/>
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="AV48" s="4">
         <v>17</v>
@@ -10596,7 +10589,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="49" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>908</v>
       </c>
@@ -10786,7 +10779,7 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="50" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:56" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6">
         <v>907</v>
       </c>
@@ -10977,11 +10970,11 @@
         <v>46142</v>
       </c>
     </row>
-    <row r="51" spans="1:56" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:56" s="13" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <v>1085</v>
       </c>
-      <c r="B51" s="33" t="s">
+      <c r="B51" s="31" t="s">
         <v>154</v>
       </c>
       <c r="C51" s="33" t="s">
@@ -11161,16 +11154,22 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" sort="0" autoFilter="0"/>
-  <autoFilter ref="A1:BD50" xr:uid="{869D9611-F0E3-4A7A-9239-9C1FA0F0C8DA}"/>
+  <autoFilter ref="A1:BD51" xr:uid="{869D9611-F0E3-4A7A-9239-9C1FA0F0C8DA}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="MXVER"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="8" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E1048196 H52:H1048196 I2:K1048196" xr:uid="{DD2A48DC-7068-4BD6-8A6F-E802386CE572}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E10 K2:K10 C14:E1048195 K14:K1048195" xr:uid="{833F6030-824F-4AAE-BA3C-131D886541AF}">
+      <formula1>shippername</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:K51 H52:K1048195 C2:E1048195" xr:uid="{DD2A48DC-7068-4BD6-8A6F-E802386CE572}">
       <formula1>AILNname</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:E10 K2:K10 K14:K1048196 C14:E1048196" xr:uid="{833F6030-824F-4AAE-BA3C-131D886541AF}">
-      <formula1>shippername</formula1>
-    </dataValidation>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check information" error="This is not a known plant, please check the spelling or enter the information in the sheet &quot;Plant_ALIN&quot;" sqref="G2:G1048196" xr:uid="{D2D52A73-EC4B-4324-8BC4-BD77EF4C5461}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Please check information" error="This is not a known plant, please check the spelling or enter the information in the sheet &quot;Plant_ALIN&quot;" sqref="G2:G1048195" xr:uid="{D2D52A73-EC4B-4324-8BC4-BD77EF4C5461}">
       <formula1>plantname</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>